<commit_message>
added fully function sorting method of books inside addBook.js and added some comments
</commit_message>
<xml_diff>
--- a/projectBookSort1.1/Backlog/Product_backlog.xlsx
+++ b/projectBookSort1.1/Backlog/Product_backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenneth/Desktop/IBA/3semester/webSpecialization/webSpecTasks/projectBookSort1.1/Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4285CC5A-E8E8-8245-AC8F-477DCBD2014D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36A1981-CB6F-7E4E-92F3-29F00C0D89F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{1D807A5E-B5B4-C94B-9F79-296DA37239DA}"/>
   </bookViews>
@@ -27,6 +27,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{FF51726F-FC36-EE4D-A0FA-42EF35E926F7}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Need to be able to add the cover image selected by user, as background-image of bookPic div
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
@@ -154,13 +178,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -313,14 +343,14 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>- Hvad med generelt at sætte classes på funktioner, så alle funktioner holdes samlet på en måde? kan man det? så man ved at alt fra denne linje og ned til næste afsnit er funktioner eks, fremfor inddeling via /*******/ </a:t>
+            <a:t>- Hvordan kan man ellers opdele sit script så det er lettere at finde frem til funktioner, uden brug af /******/ for at vise hvad der kommer herfra og ned? </a:t>
           </a:r>
           <a:br>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
           </a:br>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>- Er opdeling af script filer smartere? e.g. anvende en scriptfil til localstorage, og en til addbook, osv.?</a:t>
+            <a:t>ville det være lettere at læse og smartere hvis man evt. opdelte scripts filer? e.g. anvende en scriptfil til localstorage, og en til addbook, osv.?</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -329,14 +359,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>- optimer addBook(){} if statements = er det ikke optimalt at opdele det til sin egen funktion og så kalde den i addBook? </a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>(kunne jeg nøjes med "required" på hvert html element i stedet for if statements?)</a:t>
+            <a:t>- addBooks checkIfnfoLegit() og dets if statements , kunne det være undgået  "required" på hvert html element i stedet for if statements?</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -404,7 +427,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>- upon adding book, clear inputs</a:t>
+            <a:t>- generel optimering af syntax hvor jeg gentager mig selv, eks. sort books med deres compare funktioner, hvordan kunne de skrives smartere?</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -474,26 +497,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>MANGLER HER OG NU:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> Skjul ikke sorteret array?</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>- sorter på titel også ved change value i selector</a:t>
+            <a:t>MANGLER:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -503,6 +507,33 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
             <a:t>- tilføj billede til cover på bog ud fra input fil</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- søg efter bog info og få forslag for hver karakter der skrives i søgefeltet</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- slet en bog fra arrayet</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- ændre info i en bog</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -809,11 +840,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05A01B6-D897-4D4A-8B88-20E49C8EBA3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05A01B6-D897-4D4A-8B88-20E49C8EBA3B}">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -992,24 +1023,24 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <v>2</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="8">
-        <v>0.5</v>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1097,5 +1128,6 @@
   <autoFilter ref="A1:G16" xr:uid="{80D6975F-6C4E-46A7-AB62-2871A49CA551}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>